<commit_message>
change LED part number in BOM excel
</commit_message>
<xml_diff>
--- a/marbles/hardware_design/pcb/kicad/jlcpcb/production_files/NEW-BOM-marbles.xlsx
+++ b/marbles/hardware_design/pcb/kicad/jlcpcb/production_files/NEW-BOM-marbles.xlsx
@@ -694,10 +694,10 @@
     <t>LED_Dual_KAKA</t>
   </si>
   <si>
-    <t>C434426</t>
-  </si>
-  <si>
-    <t>20mA Colorless transparence -30℃~+85℃ Red, General Green/Yellow-Green 120° 40mW 0606  Light Emitting Diodes (LED) ROHS</t>
+    <t>C375546</t>
+  </si>
+  <si>
+    <t>20mA -40℃~+90℃ Red, General Green/Yellow-Green 120° 0805  Light Emitting Diodes (LED) ROHS</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -719,13 +719,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -744,8 +749,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -757,6 +768,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -770,7 +803,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -779,7 +812,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,43 +821,28 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -833,28 +851,58 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -864,41 +912,47 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -918,8 +972,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -938,10 +994,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -1118,11 +1174,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1131,7 +1190,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1146,19 +1205,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="2200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1408,10 +1467,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1702,7 +1761,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1983,7 +2042,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2001,912 +2060,912 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="6">
         <v>603</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" t="s" s="7">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="E3" t="s" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="A4" t="s" s="9">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="8">
+      <c r="B4" t="s" s="10">
         <v>11</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="C4" t="s" s="11">
         <v>12</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="A5" t="s" s="9">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="8">
+      <c r="B5" t="s" s="10">
         <v>14</v>
       </c>
-      <c r="C5" t="s" s="9">
+      <c r="C5" t="s" s="11">
         <v>15</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="7">
+      <c r="A6" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B6" t="s" s="8">
+      <c r="B6" t="s" s="10">
         <v>17</v>
       </c>
-      <c r="C6" t="s" s="9">
+      <c r="C6" t="s" s="11">
         <v>18</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="A7" t="s" s="9">
         <v>19</v>
       </c>
-      <c r="B7" t="s" s="8">
+      <c r="B7" t="s" s="10">
         <v>20</v>
       </c>
-      <c r="C7" t="s" s="9">
+      <c r="C7" t="s" s="11">
         <v>21</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="7">
+      <c r="A8" t="s" s="9">
         <v>22</v>
       </c>
-      <c r="B8" t="s" s="8">
+      <c r="B8" t="s" s="10">
         <v>23</v>
       </c>
-      <c r="C8" t="s" s="9">
+      <c r="C8" t="s" s="11">
         <v>24</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="7">
+      <c r="A9" t="s" s="9">
         <v>25</v>
       </c>
-      <c r="B9" t="s" s="8">
+      <c r="B9" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="C9" t="s" s="9">
+      <c r="C9" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="7">
+      <c r="A10" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B10" t="s" s="8">
+      <c r="B10" t="s" s="10">
         <v>29</v>
       </c>
-      <c r="C10" t="s" s="9">
+      <c r="C10" t="s" s="11">
         <v>30</v>
       </c>
-      <c r="D10" t="s" s="9">
+      <c r="D10" t="s" s="11">
         <v>31</v>
       </c>
-      <c r="E10" t="s" s="9">
+      <c r="E10" t="s" s="11">
         <v>32</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="7">
+      <c r="A11" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B11" t="s" s="8">
+      <c r="B11" t="s" s="10">
         <v>33</v>
       </c>
-      <c r="C11" t="s" s="9">
+      <c r="C11" t="s" s="11">
         <v>34</v>
       </c>
-      <c r="D11" t="s" s="9">
+      <c r="D11" t="s" s="11">
         <v>35</v>
       </c>
-      <c r="E11" t="s" s="9">
+      <c r="E11" t="s" s="11">
         <v>36</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="7">
+      <c r="A12" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B12" t="s" s="8">
+      <c r="B12" t="s" s="10">
         <v>37</v>
       </c>
-      <c r="C12" t="s" s="9">
+      <c r="C12" t="s" s="11">
         <v>38</v>
       </c>
-      <c r="D12" t="s" s="9">
+      <c r="D12" t="s" s="11">
         <v>39</v>
       </c>
-      <c r="E12" t="s" s="9">
+      <c r="E12" t="s" s="11">
         <v>40</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="7">
+      <c r="A13" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B13" t="s" s="8">
+      <c r="B13" t="s" s="10">
         <v>41</v>
       </c>
-      <c r="C13" t="s" s="9">
+      <c r="C13" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="D13" t="s" s="9">
+      <c r="D13" t="s" s="11">
         <v>43</v>
       </c>
-      <c r="E13" t="s" s="9">
+      <c r="E13" t="s" s="11">
         <v>44</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="7">
+      <c r="A14" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B14" t="s" s="8">
+      <c r="B14" t="s" s="10">
         <v>45</v>
       </c>
-      <c r="C14" t="s" s="9">
+      <c r="C14" t="s" s="11">
         <v>46</v>
       </c>
-      <c r="D14" t="s" s="9">
+      <c r="D14" t="s" s="11">
         <v>47</v>
       </c>
-      <c r="E14" t="s" s="9">
+      <c r="E14" t="s" s="11">
         <v>48</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="7">
+      <c r="A15" t="s" s="9">
         <v>28</v>
       </c>
-      <c r="B15" t="s" s="8">
+      <c r="B15" t="s" s="10">
         <v>49</v>
       </c>
-      <c r="C15" t="s" s="9">
+      <c r="C15" t="s" s="11">
         <v>50</v>
       </c>
-      <c r="D15" t="s" s="9">
+      <c r="D15" t="s" s="11">
         <v>51</v>
       </c>
-      <c r="E15" t="s" s="9">
+      <c r="E15" t="s" s="11">
         <v>52</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="7">
+      <c r="A16" t="s" s="9">
         <v>53</v>
       </c>
-      <c r="B16" t="s" s="8">
+      <c r="B16" t="s" s="10">
         <v>54</v>
       </c>
-      <c r="C16" t="s" s="9">
+      <c r="C16" t="s" s="11">
         <v>55</v>
       </c>
-      <c r="D16" t="s" s="9">
+      <c r="D16" t="s" s="11">
         <v>56</v>
       </c>
-      <c r="E16" t="s" s="9">
+      <c r="E16" t="s" s="11">
         <v>57</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="7">
+      <c r="A17" t="s" s="9">
         <v>58</v>
       </c>
-      <c r="B17" t="s" s="8">
+      <c r="B17" t="s" s="10">
         <v>59</v>
       </c>
-      <c r="C17" t="s" s="9">
+      <c r="C17" t="s" s="11">
         <v>60</v>
       </c>
-      <c r="D17" t="s" s="9">
+      <c r="D17" t="s" s="11">
         <v>61</v>
       </c>
-      <c r="E17" t="s" s="9">
+      <c r="E17" t="s" s="11">
         <v>62</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="7">
+      <c r="A18" t="s" s="9">
         <v>63</v>
       </c>
-      <c r="B18" t="s" s="8">
+      <c r="B18" t="s" s="10">
         <v>64</v>
       </c>
-      <c r="C18" t="s" s="9">
+      <c r="C18" t="s" s="11">
         <v>65</v>
       </c>
-      <c r="D18" t="s" s="9">
+      <c r="D18" t="s" s="11">
         <v>66</v>
       </c>
-      <c r="E18" t="s" s="9">
+      <c r="E18" t="s" s="11">
         <v>67</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="7">
+      <c r="A19" t="s" s="9">
         <v>68</v>
       </c>
-      <c r="B19" t="s" s="8">
+      <c r="B19" t="s" s="10">
         <v>69</v>
       </c>
-      <c r="C19" t="s" s="9">
+      <c r="C19" t="s" s="11">
         <v>70</v>
       </c>
-      <c r="D19" t="s" s="9">
+      <c r="D19" t="s" s="11">
         <v>71</v>
       </c>
-      <c r="E19" t="s" s="9">
+      <c r="E19" t="s" s="11">
         <v>72</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="7">
+      <c r="A20" t="s" s="9">
         <v>73</v>
       </c>
-      <c r="B20" t="s" s="8">
+      <c r="B20" t="s" s="10">
         <v>74</v>
       </c>
-      <c r="C20" t="s" s="9">
+      <c r="C20" t="s" s="11">
         <v>75</v>
       </c>
-      <c r="D20" t="s" s="9">
+      <c r="D20" t="s" s="11">
         <v>76</v>
       </c>
-      <c r="E20" t="s" s="9">
+      <c r="E20" t="s" s="11">
         <v>77</v>
       </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="7">
+      <c r="A21" t="s" s="9">
         <v>78</v>
       </c>
-      <c r="B21" t="s" s="8">
+      <c r="B21" t="s" s="10">
         <v>79</v>
       </c>
-      <c r="C21" t="s" s="9">
+      <c r="C21" t="s" s="11">
         <v>80</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="7">
+      <c r="A22" t="s" s="9">
         <v>81</v>
       </c>
-      <c r="B22" t="s" s="8">
+      <c r="B22" t="s" s="10">
         <v>82</v>
       </c>
-      <c r="C22" t="s" s="9">
+      <c r="C22" t="s" s="11">
         <v>83</v>
       </c>
-      <c r="D22" t="s" s="9">
+      <c r="D22" t="s" s="11">
         <v>84</v>
       </c>
-      <c r="E22" t="s" s="9">
+      <c r="E22" t="s" s="11">
         <v>85</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="7">
+      <c r="A23" t="s" s="9">
         <v>86</v>
       </c>
-      <c r="B23" t="s" s="8">
+      <c r="B23" t="s" s="10">
         <v>87</v>
       </c>
-      <c r="C23" t="s" s="9">
+      <c r="C23" t="s" s="11">
         <v>88</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="7">
+      <c r="A24" t="s" s="9">
         <v>89</v>
       </c>
-      <c r="B24" t="s" s="8">
+      <c r="B24" t="s" s="10">
         <v>90</v>
       </c>
-      <c r="C24" t="s" s="9">
+      <c r="C24" t="s" s="11">
         <v>91</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="7">
+      <c r="A25" t="s" s="9">
         <v>92</v>
       </c>
-      <c r="B25" t="s" s="8">
+      <c r="B25" t="s" s="10">
         <v>93</v>
       </c>
-      <c r="C25" t="s" s="9">
+      <c r="C25" t="s" s="11">
         <v>65</v>
       </c>
-      <c r="D25" t="s" s="9">
+      <c r="D25" t="s" s="11">
         <v>94</v>
       </c>
-      <c r="E25" t="s" s="9">
+      <c r="E25" t="s" s="11">
         <v>95</v>
       </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="7">
+      <c r="A26" t="s" s="9">
         <v>96</v>
       </c>
-      <c r="B26" t="s" s="8">
+      <c r="B26" t="s" s="10">
         <v>97</v>
       </c>
-      <c r="C26" t="s" s="9">
+      <c r="C26" t="s" s="11">
         <v>98</v>
       </c>
-      <c r="D26" t="s" s="9">
+      <c r="D26" t="s" s="11">
         <v>99</v>
       </c>
-      <c r="E26" t="s" s="9">
+      <c r="E26" t="s" s="11">
         <v>100</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="7">
+      <c r="A27" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B27" t="s" s="8">
+      <c r="B27" t="s" s="10">
         <v>102</v>
       </c>
-      <c r="C27" t="s" s="9">
+      <c r="C27" t="s" s="11">
         <v>103</v>
       </c>
-      <c r="D27" t="s" s="9">
+      <c r="D27" t="s" s="11">
         <v>104</v>
       </c>
-      <c r="E27" t="s" s="9">
+      <c r="E27" t="s" s="11">
         <v>105</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="7">
+      <c r="A28" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B28" t="s" s="8">
+      <c r="B28" t="s" s="10">
         <v>106</v>
       </c>
-      <c r="C28" t="s" s="9">
+      <c r="C28" t="s" s="11">
         <v>107</v>
       </c>
-      <c r="D28" t="s" s="9">
+      <c r="D28" t="s" s="11">
         <v>108</v>
       </c>
-      <c r="E28" t="s" s="9">
+      <c r="E28" t="s" s="11">
         <v>109</v>
       </c>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="7">
+      <c r="A29" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B29" t="s" s="8">
+      <c r="B29" t="s" s="10">
         <v>110</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="13">
         <v>100</v>
       </c>
-      <c r="D29" t="s" s="9">
+      <c r="D29" t="s" s="11">
         <v>111</v>
       </c>
-      <c r="E29" t="s" s="9">
+      <c r="E29" t="s" s="11">
         <v>112</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" t="s" s="7">
+      <c r="A30" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B30" t="s" s="8">
+      <c r="B30" t="s" s="10">
         <v>113</v>
       </c>
-      <c r="C30" t="s" s="9">
+      <c r="C30" t="s" s="11">
         <v>114</v>
       </c>
-      <c r="D30" t="s" s="9">
+      <c r="D30" t="s" s="11">
         <v>115</v>
       </c>
-      <c r="E30" t="s" s="9">
+      <c r="E30" t="s" s="11">
         <v>116</v>
       </c>
     </row>
     <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" t="s" s="7">
+      <c r="A31" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B31" t="s" s="8">
+      <c r="B31" t="s" s="10">
         <v>117</v>
       </c>
-      <c r="C31" t="s" s="9">
+      <c r="C31" t="s" s="11">
         <v>118</v>
       </c>
-      <c r="D31" t="s" s="9">
+      <c r="D31" t="s" s="11">
         <v>119</v>
       </c>
-      <c r="E31" t="s" s="9">
+      <c r="E31" t="s" s="11">
         <v>120</v>
       </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" t="s" s="7">
+      <c r="A32" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B32" t="s" s="8">
+      <c r="B32" t="s" s="10">
         <v>121</v>
       </c>
-      <c r="C32" t="s" s="9">
+      <c r="C32" t="s" s="11">
         <v>122</v>
       </c>
-      <c r="D32" t="s" s="9">
+      <c r="D32" t="s" s="11">
         <v>123</v>
       </c>
-      <c r="E32" t="s" s="9">
+      <c r="E32" t="s" s="11">
         <v>124</v>
       </c>
     </row>
     <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" t="s" s="7">
+      <c r="A33" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B33" t="s" s="8">
+      <c r="B33" t="s" s="10">
         <v>125</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="13">
         <v>180</v>
       </c>
-      <c r="D33" t="s" s="9">
+      <c r="D33" t="s" s="11">
         <v>126</v>
       </c>
-      <c r="E33" t="s" s="9">
+      <c r="E33" t="s" s="11">
         <v>127</v>
       </c>
     </row>
     <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" t="s" s="7">
+      <c r="A34" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B34" t="s" s="8">
+      <c r="B34" t="s" s="10">
         <v>128</v>
       </c>
-      <c r="C34" t="s" s="9">
+      <c r="C34" t="s" s="11">
         <v>129</v>
       </c>
-      <c r="D34" t="s" s="9">
+      <c r="D34" t="s" s="11">
         <v>130</v>
       </c>
-      <c r="E34" t="s" s="9">
+      <c r="E34" t="s" s="11">
         <v>131</v>
       </c>
     </row>
     <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" t="s" s="7">
+      <c r="A35" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B35" t="s" s="8">
+      <c r="B35" t="s" s="10">
         <v>132</v>
       </c>
-      <c r="C35" t="s" s="9">
+      <c r="C35" t="s" s="11">
         <v>133</v>
       </c>
-      <c r="D35" t="s" s="9">
+      <c r="D35" t="s" s="11">
         <v>134</v>
       </c>
-      <c r="E35" t="s" s="9">
+      <c r="E35" t="s" s="11">
         <v>135</v>
       </c>
     </row>
     <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" t="s" s="7">
+      <c r="A36" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B36" t="s" s="8">
+      <c r="B36" t="s" s="10">
         <v>136</v>
       </c>
-      <c r="C36" t="s" s="9">
+      <c r="C36" t="s" s="11">
         <v>137</v>
       </c>
-      <c r="D36" t="s" s="9">
+      <c r="D36" t="s" s="11">
         <v>138</v>
       </c>
-      <c r="E36" t="s" s="9">
+      <c r="E36" t="s" s="11">
         <v>139</v>
       </c>
     </row>
     <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" t="s" s="7">
+      <c r="A37" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B37" t="s" s="8">
+      <c r="B37" t="s" s="10">
         <v>140</v>
       </c>
-      <c r="C37" t="s" s="9">
+      <c r="C37" t="s" s="11">
         <v>141</v>
       </c>
-      <c r="D37" t="s" s="9">
+      <c r="D37" t="s" s="11">
         <v>142</v>
       </c>
-      <c r="E37" t="s" s="9">
+      <c r="E37" t="s" s="11">
         <v>143</v>
       </c>
     </row>
     <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" t="s" s="7">
+      <c r="A38" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B38" t="s" s="8">
+      <c r="B38" t="s" s="10">
         <v>144</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="13">
         <v>39</v>
       </c>
-      <c r="D38" t="s" s="9">
+      <c r="D38" t="s" s="11">
         <v>145</v>
       </c>
-      <c r="E38" t="s" s="9">
+      <c r="E38" t="s" s="11">
         <v>146</v>
       </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" t="s" s="7">
+      <c r="A39" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B39" t="s" s="8">
+      <c r="B39" t="s" s="10">
         <v>147</v>
       </c>
-      <c r="C39" t="s" s="9">
+      <c r="C39" t="s" s="11">
         <v>148</v>
       </c>
-      <c r="D39" t="s" s="9">
+      <c r="D39" t="s" s="11">
         <v>149</v>
       </c>
-      <c r="E39" t="s" s="9">
+      <c r="E39" t="s" s="11">
         <v>150</v>
       </c>
     </row>
     <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" t="s" s="7">
+      <c r="A40" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B40" t="s" s="8">
+      <c r="B40" t="s" s="10">
         <v>151</v>
       </c>
-      <c r="C40" t="s" s="9">
+      <c r="C40" t="s" s="11">
         <v>152</v>
       </c>
-      <c r="D40" t="s" s="9">
+      <c r="D40" t="s" s="11">
         <v>153</v>
       </c>
-      <c r="E40" t="s" s="9">
+      <c r="E40" t="s" s="11">
         <v>154</v>
       </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" t="s" s="7">
+      <c r="A41" t="s" s="9">
         <v>101</v>
       </c>
-      <c r="B41" t="s" s="8">
+      <c r="B41" t="s" s="10">
         <v>155</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="13">
         <v>680</v>
       </c>
-      <c r="D41" t="s" s="9">
+      <c r="D41" t="s" s="11">
         <v>156</v>
       </c>
-      <c r="E41" t="s" s="9">
+      <c r="E41" t="s" s="11">
         <v>157</v>
       </c>
     </row>
     <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" t="s" s="7">
+      <c r="A42" t="s" s="9">
         <v>158</v>
       </c>
-      <c r="B42" t="s" s="8">
+      <c r="B42" t="s" s="10">
         <v>159</v>
       </c>
-      <c r="C42" t="s" s="9">
+      <c r="C42" t="s" s="11">
         <v>103</v>
       </c>
-      <c r="D42" t="s" s="9">
+      <c r="D42" t="s" s="11">
         <v>160</v>
       </c>
-      <c r="E42" t="s" s="9">
+      <c r="E42" t="s" s="11">
         <v>161</v>
       </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" t="s" s="7">
+      <c r="A43" t="s" s="9">
         <v>162</v>
       </c>
-      <c r="B43" t="s" s="8">
+      <c r="B43" t="s" s="10">
         <v>163</v>
       </c>
-      <c r="C43" t="s" s="9">
+      <c r="C43" t="s" s="11">
         <v>164</v>
       </c>
-      <c r="D43" t="s" s="9">
+      <c r="D43" t="s" s="11">
         <v>165</v>
       </c>
-      <c r="E43" t="s" s="9">
+      <c r="E43" t="s" s="11">
         <v>166</v>
       </c>
     </row>
     <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" t="s" s="7">
+      <c r="A44" t="s" s="9">
         <v>167</v>
       </c>
-      <c r="B44" t="s" s="8">
+      <c r="B44" t="s" s="10">
         <v>168</v>
       </c>
-      <c r="C44" t="s" s="9">
+      <c r="C44" t="s" s="11">
         <v>169</v>
       </c>
-      <c r="D44" t="s" s="9">
+      <c r="D44" t="s" s="11">
         <v>170</v>
       </c>
-      <c r="E44" t="s" s="9">
+      <c r="E44" t="s" s="11">
         <v>171</v>
       </c>
     </row>
     <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" t="s" s="7">
+      <c r="A45" t="s" s="9">
         <v>172</v>
       </c>
-      <c r="B45" t="s" s="8">
+      <c r="B45" t="s" s="10">
         <v>173</v>
       </c>
-      <c r="C45" t="s" s="9">
+      <c r="C45" t="s" s="11">
         <v>174</v>
       </c>
-      <c r="D45" t="s" s="9">
+      <c r="D45" t="s" s="11">
         <v>175</v>
       </c>
-      <c r="E45" t="s" s="9">
+      <c r="E45" t="s" s="11">
         <v>176</v>
       </c>
     </row>
     <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" t="s" s="7">
+      <c r="A46" t="s" s="9">
         <v>177</v>
       </c>
-      <c r="B46" t="s" s="8">
+      <c r="B46" t="s" s="10">
         <v>178</v>
       </c>
-      <c r="C46" t="s" s="9">
+      <c r="C46" t="s" s="11">
         <v>179</v>
       </c>
-      <c r="D46" t="s" s="9">
+      <c r="D46" t="s" s="11">
         <v>180</v>
       </c>
-      <c r="E46" t="s" s="9">
+      <c r="E46" t="s" s="11">
         <v>181</v>
       </c>
     </row>
     <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" t="s" s="7">
+      <c r="A47" t="s" s="9">
         <v>182</v>
       </c>
-      <c r="B47" t="s" s="8">
+      <c r="B47" t="s" s="10">
         <v>183</v>
       </c>
-      <c r="C47" t="s" s="9">
+      <c r="C47" t="s" s="11">
         <v>184</v>
       </c>
-      <c r="D47" t="s" s="9">
+      <c r="D47" t="s" s="11">
         <v>185</v>
       </c>
-      <c r="E47" t="s" s="9">
+      <c r="E47" t="s" s="11">
         <v>186</v>
       </c>
     </row>
     <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" t="s" s="7">
+      <c r="A48" t="s" s="9">
         <v>187</v>
       </c>
-      <c r="B48" t="s" s="8">
+      <c r="B48" t="s" s="10">
         <v>188</v>
       </c>
-      <c r="C48" t="s" s="9">
+      <c r="C48" t="s" s="11">
         <v>189</v>
       </c>
-      <c r="D48" t="s" s="9">
+      <c r="D48" t="s" s="11">
         <v>190</v>
       </c>
-      <c r="E48" t="s" s="9">
+      <c r="E48" t="s" s="11">
         <v>191</v>
       </c>
     </row>
     <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" t="s" s="7">
+      <c r="A49" t="s" s="9">
         <v>192</v>
       </c>
-      <c r="B49" t="s" s="8">
+      <c r="B49" t="s" s="10">
         <v>193</v>
       </c>
-      <c r="C49" t="s" s="9">
+      <c r="C49" t="s" s="11">
         <v>194</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" t="s" s="7">
+      <c r="A50" t="s" s="9">
         <v>195</v>
       </c>
-      <c r="B50" t="s" s="8">
+      <c r="B50" t="s" s="10">
         <v>196</v>
       </c>
-      <c r="C50" t="s" s="9">
+      <c r="C50" t="s" s="11">
         <v>197</v>
       </c>
-      <c r="D50" t="s" s="9">
+      <c r="D50" t="s" s="11">
         <v>198</v>
       </c>
-      <c r="E50" t="s" s="9">
+      <c r="E50" t="s" s="11">
         <v>199</v>
       </c>
     </row>
     <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" t="s" s="7">
+      <c r="A51" t="s" s="9">
         <v>200</v>
       </c>
-      <c r="B51" t="s" s="8">
+      <c r="B51" t="s" s="10">
         <v>201</v>
       </c>
-      <c r="C51" t="s" s="9">
+      <c r="C51" t="s" s="11">
         <v>202</v>
       </c>
-      <c r="D51" t="s" s="9">
+      <c r="D51" t="s" s="11">
         <v>203</v>
       </c>
-      <c r="E51" t="s" s="9">
+      <c r="E51" t="s" s="11">
         <v>204</v>
       </c>
     </row>
     <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" t="s" s="7">
+      <c r="A52" t="s" s="9">
         <v>205</v>
       </c>
-      <c r="B52" t="s" s="8">
+      <c r="B52" t="s" s="10">
         <v>206</v>
       </c>
-      <c r="C52" t="s" s="9">
+      <c r="C52" t="s" s="11">
         <v>207</v>
       </c>
-      <c r="D52" t="s" s="9">
+      <c r="D52" t="s" s="11">
         <v>208</v>
       </c>
-      <c r="E52" t="s" s="9">
+      <c r="E52" t="s" s="11">
         <v>209</v>
       </c>
     </row>
     <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" t="s" s="7">
+      <c r="A53" t="s" s="9">
         <v>205</v>
       </c>
-      <c r="B53" t="s" s="8">
+      <c r="B53" t="s" s="10">
         <v>210</v>
       </c>
-      <c r="C53" t="s" s="9">
+      <c r="C53" t="s" s="11">
         <v>211</v>
       </c>
-      <c r="D53" t="s" s="9">
+      <c r="D53" t="s" s="11">
         <v>212</v>
       </c>
-      <c r="E53" t="s" s="9">
+      <c r="E53" t="s" s="11">
         <v>213</v>
       </c>
     </row>
     <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" t="s" s="7">
+      <c r="A54" t="s" s="9">
         <v>205</v>
       </c>
-      <c r="B54" t="s" s="8">
+      <c r="B54" t="s" s="10">
         <v>214</v>
       </c>
-      <c r="C54" t="s" s="9">
+      <c r="C54" t="s" s="11">
         <v>215</v>
       </c>
-      <c r="D54" t="s" s="9">
+      <c r="D54" t="s" s="11">
         <v>216</v>
       </c>
-      <c r="E54" t="s" s="9">
+      <c r="E54" t="s" s="11">
         <v>217</v>
       </c>
     </row>
     <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" t="s" s="7">
+      <c r="A55" t="s" s="9">
         <v>218</v>
       </c>
-      <c r="B55" t="s" s="8">
+      <c r="B55" t="s" s="10">
         <v>219</v>
       </c>
-      <c r="C55" t="s" s="9">
+      <c r="C55" t="s" s="11">
         <v>220</v>
       </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
     </row>
     <row r="56" ht="20.05" customHeight="1">
-      <c r="A56" t="s" s="7">
+      <c r="A56" t="s" s="9">
         <v>221</v>
       </c>
-      <c r="B56" t="s" s="8">
+      <c r="B56" t="s" s="10">
         <v>222</v>
       </c>
-      <c r="C56" t="s" s="9">
+      <c r="C56" t="s" s="11">
         <v>223</v>
       </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
     </row>
     <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" t="s" s="7">
+      <c r="A57" t="s" s="9">
         <v>224</v>
       </c>
-      <c r="B57" t="s" s="8">
+      <c r="B57" t="s" s="10">
         <v>225</v>
       </c>
-      <c r="C57" t="s" s="9">
+      <c r="C57" t="s" s="11">
         <v>226</v>
       </c>
-      <c r="D57" t="s" s="9">
+      <c r="D57" t="s" s="11">
         <v>227</v>
       </c>
-      <c r="E57" t="s" s="9">
+      <c r="E57" t="s" s="11">
         <v>228</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change same resistors in BOM excel
</commit_message>
<xml_diff>
--- a/marbles/hardware_design/pcb/kicad/jlcpcb/production_files/NEW-BOM-marbles.xlsx
+++ b/marbles/hardware_design/pcb/kicad/jlcpcb/production_files/NEW-BOM-marbles.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="227">
   <si>
     <t>NEW-BOM-marbles</t>
   </si>
@@ -445,13 +445,16 @@
     <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 33kΩ 0402  Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
+    <t>R0603</t>
+  </si>
+  <si>
     <t>R1,R5</t>
   </si>
   <si>
-    <t>C25110</t>
-  </si>
-  <si>
-    <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 39Ω 0402  Chip Resistor - Surface Mount ROHS</t>
+    <t>C21190</t>
+  </si>
+  <si>
+    <t>1/10W Thick Film Resistors 75V ±1% ±100ppm/℃ -55℃~+155℃ 1kΩ 0603  Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
     <t>R49,R50,R75</t>
@@ -487,16 +490,7 @@
     <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 680Ω 0402  Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
-    <t>R0603</t>
-  </si>
-  <si>
     <t>R45,R46,R62,R63,R85,R86,R87</t>
-  </si>
-  <si>
-    <t>C21190</t>
-  </si>
-  <si>
-    <t>1/10W Thick Film Resistors 75V ±1% ±100ppm/℃ -55℃~+155℃ 1kΩ 0603  Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
     <t>SO-14_3.9x8.65mm_P1.27mm</t>
@@ -2643,19 +2637,19 @@
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="9">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s" s="10">
-        <v>144</v>
-      </c>
-      <c r="C38" s="13">
-        <v>39</v>
+        <v>145</v>
+      </c>
+      <c r="C38" t="s" s="11">
+        <v>103</v>
       </c>
       <c r="D38" t="s" s="11">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E38" t="s" s="11">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
@@ -2663,16 +2657,16 @@
         <v>101</v>
       </c>
       <c r="B39" t="s" s="10">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s" s="11">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D39" t="s" s="11">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E39" t="s" s="11">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" ht="20.05" customHeight="1">
@@ -2680,16 +2674,16 @@
         <v>101</v>
       </c>
       <c r="B40" t="s" s="10">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s" s="11">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D40" t="s" s="11">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s" s="11">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
@@ -2697,21 +2691,21 @@
         <v>101</v>
       </c>
       <c r="B41" t="s" s="10">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C41" s="13">
         <v>680</v>
       </c>
       <c r="D41" t="s" s="11">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E41" t="s" s="11">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" t="s" s="9">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B42" t="s" s="10">
         <v>159</v>
@@ -2720,253 +2714,253 @@
         <v>103</v>
       </c>
       <c r="D42" t="s" s="11">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="E42" t="s" s="11">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="9">
+        <v>160</v>
+      </c>
+      <c r="B43" t="s" s="10">
+        <v>161</v>
+      </c>
+      <c r="C43" t="s" s="11">
         <v>162</v>
       </c>
-      <c r="B43" t="s" s="10">
+      <c r="D43" t="s" s="11">
         <v>163</v>
       </c>
-      <c r="C43" t="s" s="11">
+      <c r="E43" t="s" s="11">
         <v>164</v>
-      </c>
-      <c r="D43" t="s" s="11">
-        <v>165</v>
-      </c>
-      <c r="E43" t="s" s="11">
-        <v>166</v>
       </c>
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="9">
+        <v>165</v>
+      </c>
+      <c r="B44" t="s" s="10">
+        <v>166</v>
+      </c>
+      <c r="C44" t="s" s="11">
         <v>167</v>
       </c>
-      <c r="B44" t="s" s="10">
+      <c r="D44" t="s" s="11">
         <v>168</v>
       </c>
-      <c r="C44" t="s" s="11">
+      <c r="E44" t="s" s="11">
         <v>169</v>
-      </c>
-      <c r="D44" t="s" s="11">
-        <v>170</v>
-      </c>
-      <c r="E44" t="s" s="11">
-        <v>171</v>
       </c>
     </row>
     <row r="45" ht="20.05" customHeight="1">
       <c r="A45" t="s" s="9">
+        <v>170</v>
+      </c>
+      <c r="B45" t="s" s="10">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s" s="11">
         <v>172</v>
       </c>
-      <c r="B45" t="s" s="10">
+      <c r="D45" t="s" s="11">
         <v>173</v>
       </c>
-      <c r="C45" t="s" s="11">
+      <c r="E45" t="s" s="11">
         <v>174</v>
-      </c>
-      <c r="D45" t="s" s="11">
-        <v>175</v>
-      </c>
-      <c r="E45" t="s" s="11">
-        <v>176</v>
       </c>
     </row>
     <row r="46" ht="20.05" customHeight="1">
       <c r="A46" t="s" s="9">
+        <v>175</v>
+      </c>
+      <c r="B46" t="s" s="10">
+        <v>176</v>
+      </c>
+      <c r="C46" t="s" s="11">
         <v>177</v>
       </c>
-      <c r="B46" t="s" s="10">
+      <c r="D46" t="s" s="11">
         <v>178</v>
       </c>
-      <c r="C46" t="s" s="11">
+      <c r="E46" t="s" s="11">
         <v>179</v>
-      </c>
-      <c r="D46" t="s" s="11">
-        <v>180</v>
-      </c>
-      <c r="E46" t="s" s="11">
-        <v>181</v>
       </c>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="9">
+        <v>180</v>
+      </c>
+      <c r="B47" t="s" s="10">
+        <v>181</v>
+      </c>
+      <c r="C47" t="s" s="11">
         <v>182</v>
       </c>
-      <c r="B47" t="s" s="10">
+      <c r="D47" t="s" s="11">
         <v>183</v>
       </c>
-      <c r="C47" t="s" s="11">
+      <c r="E47" t="s" s="11">
         <v>184</v>
-      </c>
-      <c r="D47" t="s" s="11">
-        <v>185</v>
-      </c>
-      <c r="E47" t="s" s="11">
-        <v>186</v>
       </c>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="9">
+        <v>185</v>
+      </c>
+      <c r="B48" t="s" s="10">
+        <v>186</v>
+      </c>
+      <c r="C48" t="s" s="11">
         <v>187</v>
       </c>
-      <c r="B48" t="s" s="10">
+      <c r="D48" t="s" s="11">
         <v>188</v>
       </c>
-      <c r="C48" t="s" s="11">
+      <c r="E48" t="s" s="11">
         <v>189</v>
-      </c>
-      <c r="D48" t="s" s="11">
-        <v>190</v>
-      </c>
-      <c r="E48" t="s" s="11">
-        <v>191</v>
       </c>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="9">
+        <v>190</v>
+      </c>
+      <c r="B49" t="s" s="10">
+        <v>191</v>
+      </c>
+      <c r="C49" t="s" s="11">
         <v>192</v>
-      </c>
-      <c r="B49" t="s" s="10">
-        <v>193</v>
-      </c>
-      <c r="C49" t="s" s="11">
-        <v>194</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" t="s" s="9">
+        <v>193</v>
+      </c>
+      <c r="B50" t="s" s="10">
+        <v>194</v>
+      </c>
+      <c r="C50" t="s" s="11">
         <v>195</v>
       </c>
-      <c r="B50" t="s" s="10">
+      <c r="D50" t="s" s="11">
         <v>196</v>
       </c>
-      <c r="C50" t="s" s="11">
+      <c r="E50" t="s" s="11">
         <v>197</v>
-      </c>
-      <c r="D50" t="s" s="11">
-        <v>198</v>
-      </c>
-      <c r="E50" t="s" s="11">
-        <v>199</v>
       </c>
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="9">
+        <v>198</v>
+      </c>
+      <c r="B51" t="s" s="10">
+        <v>199</v>
+      </c>
+      <c r="C51" t="s" s="11">
         <v>200</v>
       </c>
-      <c r="B51" t="s" s="10">
+      <c r="D51" t="s" s="11">
         <v>201</v>
       </c>
-      <c r="C51" t="s" s="11">
+      <c r="E51" t="s" s="11">
         <v>202</v>
-      </c>
-      <c r="D51" t="s" s="11">
-        <v>203</v>
-      </c>
-      <c r="E51" t="s" s="11">
-        <v>204</v>
       </c>
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="9">
+        <v>203</v>
+      </c>
+      <c r="B52" t="s" s="10">
+        <v>204</v>
+      </c>
+      <c r="C52" t="s" s="11">
         <v>205</v>
       </c>
-      <c r="B52" t="s" s="10">
+      <c r="D52" t="s" s="11">
         <v>206</v>
       </c>
-      <c r="C52" t="s" s="11">
+      <c r="E52" t="s" s="11">
         <v>207</v>
-      </c>
-      <c r="D52" t="s" s="11">
-        <v>208</v>
-      </c>
-      <c r="E52" t="s" s="11">
-        <v>209</v>
       </c>
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="9">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B53" t="s" s="10">
+        <v>208</v>
+      </c>
+      <c r="C53" t="s" s="11">
+        <v>209</v>
+      </c>
+      <c r="D53" t="s" s="11">
         <v>210</v>
       </c>
-      <c r="C53" t="s" s="11">
+      <c r="E53" t="s" s="11">
         <v>211</v>
-      </c>
-      <c r="D53" t="s" s="11">
-        <v>212</v>
-      </c>
-      <c r="E53" t="s" s="11">
-        <v>213</v>
       </c>
     </row>
     <row r="54" ht="20.05" customHeight="1">
       <c r="A54" t="s" s="9">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B54" t="s" s="10">
+        <v>212</v>
+      </c>
+      <c r="C54" t="s" s="11">
+        <v>213</v>
+      </c>
+      <c r="D54" t="s" s="11">
         <v>214</v>
       </c>
-      <c r="C54" t="s" s="11">
+      <c r="E54" t="s" s="11">
         <v>215</v>
-      </c>
-      <c r="D54" t="s" s="11">
-        <v>216</v>
-      </c>
-      <c r="E54" t="s" s="11">
-        <v>217</v>
       </c>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="9">
+        <v>216</v>
+      </c>
+      <c r="B55" t="s" s="10">
+        <v>217</v>
+      </c>
+      <c r="C55" t="s" s="11">
         <v>218</v>
-      </c>
-      <c r="B55" t="s" s="10">
-        <v>219</v>
-      </c>
-      <c r="C55" t="s" s="11">
-        <v>220</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
     </row>
     <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="9">
+        <v>219</v>
+      </c>
+      <c r="B56" t="s" s="10">
+        <v>220</v>
+      </c>
+      <c r="C56" t="s" s="11">
         <v>221</v>
-      </c>
-      <c r="B56" t="s" s="10">
-        <v>222</v>
-      </c>
-      <c r="C56" t="s" s="11">
-        <v>223</v>
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
     </row>
     <row r="57" ht="20.05" customHeight="1">
       <c r="A57" t="s" s="9">
+        <v>222</v>
+      </c>
+      <c r="B57" t="s" s="10">
+        <v>223</v>
+      </c>
+      <c r="C57" t="s" s="11">
         <v>224</v>
       </c>
-      <c r="B57" t="s" s="10">
+      <c r="D57" t="s" s="11">
         <v>225</v>
       </c>
-      <c r="C57" t="s" s="11">
+      <c r="E57" t="s" s="11">
         <v>226</v>
-      </c>
-      <c r="D57" t="s" s="11">
-        <v>227</v>
-      </c>
-      <c r="E57" t="s" s="11">
-        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
marbles bom: use correct lm4040 and new led resistors
</commit_message>
<xml_diff>
--- a/marbles/hardware_design/pcb/kicad/jlcpcb/production_files/NEW-BOM-marbles.xlsx
+++ b/marbles/hardware_design/pcb/kicad/jlcpcb/production_files/NEW-BOM-marbles.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="229">
   <si>
     <t>NEW-BOM-marbles</t>
   </si>
@@ -241,10 +241,10 @@
     <t>LM4040B10</t>
   </si>
   <si>
-    <t>C129965</t>
-  </si>
-  <si>
-    <t>10V -40℃~+85℃@(TA) ±0.1% 103μA 15mA 100ppm/℃ Fixed SOT-23(SOT-23-3)  Voltage References ROHS</t>
+    <t>C701887</t>
+  </si>
+  <si>
+    <t>±0.5% 15mA Fixed SOT-23-3 Voltage References ROHS</t>
   </si>
   <si>
     <t>FIDUCIAL-1X2</t>
@@ -451,46 +451,52 @@
     <t>R1,R5</t>
   </si>
   <si>
+    <t>C23228</t>
+  </si>
+  <si>
+    <t>100mW Thick Film Resistors ±100ppm/℃ ±1% 680Ω 0603  Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>R49,R50,R75</t>
+  </si>
+  <si>
+    <t>39k</t>
+  </si>
+  <si>
+    <t>C25783</t>
+  </si>
+  <si>
+    <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 39kΩ 0402  Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>R51,R52,R69</t>
+  </si>
+  <si>
+    <t>56k</t>
+  </si>
+  <si>
+    <t>C25796</t>
+  </si>
+  <si>
+    <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 56kΩ 0402  Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>R78,R79,R80,R81</t>
+  </si>
+  <si>
+    <t>C25130</t>
+  </si>
+  <si>
+    <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 680Ω 0402  Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>R45,R46,R62,R63,R85,R86,R87</t>
+  </si>
+  <si>
     <t>C21190</t>
   </si>
   <si>
     <t>1/10W Thick Film Resistors 75V ±1% ±100ppm/℃ -55℃~+155℃ 1kΩ 0603  Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>R49,R50,R75</t>
-  </si>
-  <si>
-    <t>39k</t>
-  </si>
-  <si>
-    <t>C25783</t>
-  </si>
-  <si>
-    <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 39kΩ 0402  Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>R51,R52,R69</t>
-  </si>
-  <si>
-    <t>56k</t>
-  </si>
-  <si>
-    <t>C25796</t>
-  </si>
-  <si>
-    <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 56kΩ 0402  Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>R78,R79,R80,R81</t>
-  </si>
-  <si>
-    <t>C25130</t>
-  </si>
-  <si>
-    <t>1/16W Thick Film Resistors 50V ±1% ±100ppm/℃ -55℃~+155℃ 680Ω 0402  Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>R45,R46,R62,R63,R85,R86,R87</t>
   </si>
   <si>
     <t>SO-14_3.9x8.65mm_P1.27mm</t>
@@ -750,7 +756,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -900,13 +906,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -945,6 +977,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
@@ -2351,10 +2389,10 @@
       <c r="C20" t="s" s="11">
         <v>75</v>
       </c>
-      <c r="D20" t="s" s="11">
+      <c r="D20" t="s" s="13">
         <v>76</v>
       </c>
-      <c r="E20" t="s" s="11">
+      <c r="E20" t="s" s="14">
         <v>77</v>
       </c>
     </row>
@@ -2489,7 +2527,7 @@
       <c r="B29" t="s" s="10">
         <v>110</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="15">
         <v>100</v>
       </c>
       <c r="D29" t="s" s="11">
@@ -2557,7 +2595,7 @@
       <c r="B33" t="s" s="10">
         <v>125</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="15">
         <v>180</v>
       </c>
       <c r="D33" t="s" s="11">
@@ -2693,7 +2731,7 @@
       <c r="B41" t="s" s="10">
         <v>156</v>
       </c>
-      <c r="C41" s="13">
+      <c r="C41" s="15">
         <v>680</v>
       </c>
       <c r="D41" t="s" s="11">
@@ -2714,253 +2752,253 @@
         <v>103</v>
       </c>
       <c r="D42" t="s" s="11">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="E42" t="s" s="11">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="9">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B43" t="s" s="10">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s" s="11">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D43" t="s" s="11">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E43" t="s" s="11">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="9">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B44" t="s" s="10">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C44" t="s" s="11">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D44" t="s" s="11">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E44" t="s" s="11">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" ht="20.05" customHeight="1">
       <c r="A45" t="s" s="9">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B45" t="s" s="10">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C45" t="s" s="11">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D45" t="s" s="11">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E45" t="s" s="11">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" ht="20.05" customHeight="1">
       <c r="A46" t="s" s="9">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B46" t="s" s="10">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C46" t="s" s="11">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D46" t="s" s="11">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E46" t="s" s="11">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="9">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B47" t="s" s="10">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C47" t="s" s="11">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D47" t="s" s="11">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E47" t="s" s="11">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="9">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B48" t="s" s="10">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C48" t="s" s="11">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D48" t="s" s="11">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E48" t="s" s="11">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="9">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B49" t="s" s="10">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C49" t="s" s="11">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" t="s" s="9">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B50" t="s" s="10">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C50" t="s" s="11">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D50" t="s" s="11">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E50" t="s" s="11">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="9">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B51" t="s" s="10">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C51" t="s" s="11">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D51" t="s" s="11">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E51" t="s" s="11">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="9">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B52" t="s" s="10">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C52" t="s" s="11">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D52" t="s" s="11">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="E52" t="s" s="11">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="9">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B53" t="s" s="10">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C53" t="s" s="11">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D53" t="s" s="11">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E53" t="s" s="11">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" ht="20.05" customHeight="1">
       <c r="A54" t="s" s="9">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B54" t="s" s="10">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C54" t="s" s="11">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D54" t="s" s="11">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E54" t="s" s="11">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="9">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B55" t="s" s="10">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C55" t="s" s="11">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
     </row>
     <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="9">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B56" t="s" s="10">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C56" t="s" s="11">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
     </row>
     <row r="57" ht="20.05" customHeight="1">
       <c r="A57" t="s" s="9">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B57" t="s" s="10">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C57" t="s" s="11">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D57" t="s" s="11">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E57" t="s" s="11">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>